<commit_message>
Fix Dockerfile, enhance 78 rules
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes78/delphes78.xlsx
+++ b/runtime/apps/delphes78/delphes78.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes78/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CBEDA6-F794-824E-B028-D182F72FEC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70C16BE9-08D9-F647-8F6E-DED35594F450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,9 +169,6 @@
     <t>Le demandeur est un stagiaire associé en profession médicale</t>
   </si>
   <si>
-    <t>Le demandeur a des difficultés pour naviguer sur le site de l'ANEF ou pour créer son compte ANEF</t>
-  </si>
-  <si>
     <t>Le demandeur souhaite déclarer un changement de statut d'étudiant à salarié</t>
   </si>
   <si>
@@ -1577,6 +1574,9 @@
     <t>15/09/2025</t>
   </si>
   <si>
+    <t>Le demandeur a des difficultés pour naviguer sur le site de l'ANEF ou pour créer son compte ANEF. Le site de l'ANEF plante ou ne permet pas à l'usager de naviguer correctement. Le site affiche un message d'erreur. L'usager tombe sur un bug.</t>
+  </si>
+  <si>
     <t>pref-delphes-sejour@yvelines.gouv.fr,pref-delphes-asile@yvelines.gouv.fr</t>
   </si>
 </sst>
@@ -1584,7 +1584,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1649,6 +1649,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0066CC"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1745,7 +1753,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1814,6 +1822,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -2116,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="B12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2132,17 +2141,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2150,10 +2159,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>6</v>
@@ -2164,13 +2173,13 @@
     </row>
     <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -2181,13 +2190,13 @@
     </row>
     <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -2198,13 +2207,13 @@
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -2215,13 +2224,13 @@
     </row>
     <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -2232,13 +2241,13 @@
     </row>
     <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -2249,13 +2258,13 @@
     </row>
     <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -2266,13 +2275,13 @@
     </row>
     <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
@@ -2283,13 +2292,13 @@
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
@@ -2300,13 +2309,13 @@
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
@@ -2317,13 +2326,13 @@
     </row>
     <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -2334,13 +2343,13 @@
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -2349,83 +2358,83 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>38</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>23</v>
@@ -2436,13 +2445,13 @@
     </row>
     <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>24</v>
@@ -2453,13 +2462,13 @@
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
@@ -2470,172 +2479,172 @@
     </row>
     <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D25" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D25" s="23" t="s">
+      <c r="E25" s="28" t="s">
         <v>347</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="D26" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>390</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D27" s="28" t="s">
-        <v>389</v>
-      </c>
-      <c r="E27" s="28" t="s">
+      <c r="C28" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="E28" s="28" t="s">
         <v>392</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A28" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>388</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="D29" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>450</v>
-      </c>
       <c r="D33" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="E33" s="34" t="s">
         <v>447</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -2684,79 +2693,79 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2814,52 +2823,52 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>465</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
@@ -2868,22 +2877,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{EA35456F-8910-A447-A530-A1B5920653C2}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{F76A545D-B594-2649-A1C1-E5F1CD1C7B5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2909,84 +2917,84 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>127</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="365" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>342</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
+        <v>395</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>396</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="C5" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="29" t="s">
         <v>398</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>399</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -3034,288 +3042,288 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>340</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3342,7 +3350,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3350,288 +3358,288 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>122</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>230</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>275</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>275</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>275</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="21" t="s">
         <v>283</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3671,19 +3679,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3720,64 +3728,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -3804,123 +3812,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>435</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>438</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>460</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -3947,89 +3955,89 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>374</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -4071,796 +4079,796 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="K3" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q4" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="O5" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q6" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>139</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L8" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q8" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>108</v>
-      </c>
       <c r="I9" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>232</v>
-      </c>
       <c r="M10" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>294</v>
-      </c>
       <c r="K12" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="N13" t="s">
         <v>367</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>366</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="L13" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="N13" t="s">
-        <v>368</v>
-      </c>
       <c r="O13" s="25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M14" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="N14" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="M14" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="N14" s="7" t="s">
+      <c r="O14" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="O14" s="7" t="s">
-        <v>380</v>
-      </c>
       <c r="P14" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M15" t="s">
+        <v>350</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="M15" t="s">
-        <v>351</v>
-      </c>
-      <c r="N15" s="7" t="s">
+      <c r="O15" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="O15" s="7" t="s">
-        <v>385</v>
-      </c>
       <c r="P15" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -4868,72 +4876,72 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M16" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="N16" s="33" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L17" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q17" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4993,19 +5001,19 @@
     </row>
     <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -5032,68 +5040,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update form handling and improve navigation links across components
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes78/delphes78.xlsx
+++ b/runtime/apps/delphes78/delphes78.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes78/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023AE33D-458C-E34E-9F95-B3C6EDE0CE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579EECDD-EB08-B341-8C64-DC949B3DDB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -2086,7 +2086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -3944,8 +3944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4022,37 +4022,37 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>102</v>
+        <v>218</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>225</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>450</v>
+        <v>88</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>79</v>
+        <v>272</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>217</v>
@@ -4070,21 +4070,21 @@
         <v>69</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>217</v>
@@ -4095,14 +4095,14 @@
       <c r="G3" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>225</v>
+      <c r="H3" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>225</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>65</v>
+        <v>450</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>79</v>
@@ -4340,34 +4340,34 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>58</v>
+        <v>277</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>132</v>
+        <v>278</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>133</v>
+        <v>279</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>105</v>
+        <v>217</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>225</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>88</v>
+        <v>323</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>280</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>272</v>
@@ -4375,67 +4375,57 @@
       <c r="L8" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="M8" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="O8" s="14" t="s">
+      <c r="M8" t="s">
+        <v>337</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="O8" s="8" t="s">
         <v>225</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q8" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>225</v>
-      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
         <v>272</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>42</v>
+      <c r="M9" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>403</v>
       </c>
       <c r="P9" s="7" t="s">
         <v>70</v>
@@ -4446,16 +4436,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>217</v>
@@ -4479,16 +4469,16 @@
         <v>272</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>225</v>
+        <v>217</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="P10" s="7" t="s">
         <v>70</v>
@@ -4499,16 +4489,16 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>217</v>
@@ -4532,16 +4522,16 @@
         <v>272</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>195</v>
+        <v>218</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="P11" s="7" t="s">
         <v>70</v>
@@ -4552,19 +4542,19 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>277</v>
+        <v>367</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>278</v>
+        <v>368</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>279</v>
+        <v>369</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>225</v>
@@ -4572,14 +4562,14 @@
       <c r="G12" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>225</v>
+      <c r="H12" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>323</v>
+        <v>225</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>280</v>
+        <v>225</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>272</v>
@@ -4590,11 +4580,11 @@
       <c r="M12" t="s">
         <v>337</v>
       </c>
-      <c r="N12" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>225</v>
+      <c r="N12" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>371</v>
       </c>
       <c r="P12" s="7" t="s">
         <v>70</v>
@@ -4604,35 +4594,50 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
-        <v>351</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>353</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>352</v>
-      </c>
-      <c r="E13" s="26" t="s">
+      <c r="A13" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>218</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="L13" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>338</v>
-      </c>
-      <c r="N13" t="s">
-        <v>354</v>
-      </c>
-      <c r="O13" s="25" t="s">
-        <v>402</v>
+      <c r="L13" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>366</v>
       </c>
       <c r="P13" s="7" t="s">
         <v>70</v>
@@ -4641,21 +4646,21 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>362</v>
+        <v>60</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>99</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>363</v>
+        <v>135</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>364</v>
+        <v>101</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>225</v>
@@ -4678,14 +4683,14 @@
       <c r="L14" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="M14" s="27" t="s">
-        <v>336</v>
+      <c r="M14" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>365</v>
+        <v>202</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>366</v>
+        <v>42</v>
       </c>
       <c r="P14" s="7" t="s">
         <v>70</v>
@@ -4696,92 +4701,81 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>367</v>
+        <v>440</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>368</v>
+        <v>442</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>369</v>
+        <v>441</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>102</v>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="J15" s="14" t="s">
-        <v>225</v>
-      </c>
+      <c r="J15" s="8"/>
       <c r="K15" s="8" t="s">
         <v>272</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="M15" t="s">
-        <v>337</v>
+      <c r="M15" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>370</v>
+        <v>442</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>371</v>
+        <v>441</v>
       </c>
       <c r="P15" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>399</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="C16" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="E16" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
       <c r="K16" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="M16" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="N16" s="33" t="s">
-        <v>404</v>
+      <c r="L16" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="N16" t="s">
+        <v>354</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="P16" s="7" t="s">
         <v>70</v>
@@ -4792,49 +4786,55 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>440</v>
+        <v>63</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>442</v>
+        <v>128</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>441</v>
+        <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+        <v>217</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>225</v>
+      </c>
       <c r="H17" s="14" t="s">
         <v>225</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="J17" s="8"/>
+      <c r="J17" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="K17" s="8" t="s">
-        <v>272</v>
+        <v>79</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="M17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>441</v>
+      <c r="M17" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add scripts for processing emails and testing analysis API
- Implemented `process_emails_tests.py` to read an Excel file, analyze email texts using an external API, and save results with timestamps.
- Added functions for backend health checks, text analysis, and field value creation from DataFrame rows.
- Created a command-line interface for specifying input/output files and API parameters.
- Developed `test_analysis.py` to test the analysis API endpoint, including checks for backend availability, application existence, and LLM configuration.
- Enhanced error handling and logging for better debugging and user feedback.
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes78/delphes78.xlsx
+++ b/runtime/apps/delphes78/delphes78.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes78/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579EECDD-EB08-B341-8C64-DC949B3DDB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A07954-8076-0D4F-B613-57D919837D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="459">
   <si>
     <t>Parameter</t>
   </si>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>smtp.gmail.com</t>
   </si>
   <si>
     <t>smtp_port</t>
@@ -904,12 +901,6 @@
 Sans action dans les prochains jours, il risquera de perdre son travail.
 Je vous remercie par avance et vous prie de noter l'urgence. Il risque son emploi, c'est donc très important.
 Monsieur C aimerait, par ailleurs, faire une demande d'Asile à la France.</t>
-  </si>
-  <si>
-    <t>Athena.Delphes@gmail.com</t>
-  </si>
-  <si>
-    <t>tubd yhuh fgiq hqrs</t>
   </si>
   <si>
     <t>statut</t>
@@ -1540,12 +1531,42 @@
   <si>
     <t>pref-delphes-sejour@yvelines.gouv.fr,pref-delphes-asile@yvelines.gouv.fr</t>
   </si>
+  <si>
+    <t>For Gmail with Athena.Delphes@gmail.com, use: tubd yhuh fgiq hqrs
+For Scaleway TEM: 64bc46a2-51f2-4152-9611-ddea51ad0709</t>
+  </si>
+  <si>
+    <t>64bc46a2-51f2-4152-9611-ddea51ad0709</t>
+  </si>
+  <si>
+    <t>For Google : smtp.gmail.com
+For Scaleway TEM: smtp.tem.scaleway.com</t>
+  </si>
+  <si>
+    <t>smtp.tem.scaleway.com</t>
+  </si>
+  <si>
+    <t>This is the TEM Project Id (for Scaleway)</t>
+  </si>
+  <si>
+    <t>59c350ec-8be5-4b8b-8a4c-93db7f9690b3</t>
+  </si>
+  <si>
+    <t>smtp_username</t>
+  </si>
+  <si>
+    <t>For Gmail: Athena.Delphes@gmail.com
+For Scaleway TEM: ne-pas-repondre@athenadecisions.ai or noreply@athenadecisions.ai</t>
+  </si>
+  <si>
+    <t>ne-pas-repondre@mail.athenadecisions.ai</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1621,6 +1642,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1714,7 +1741,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1784,6 +1811,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -2102,12 +2130,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2120,10 +2148,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>6</v>
@@ -2137,10 +2165,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -2154,10 +2182,10 @@
         <v>38</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -2168,13 +2196,13 @@
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -2188,10 +2216,10 @@
         <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -2205,10 +2233,10 @@
         <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -2219,13 +2247,13 @@
     </row>
     <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -2236,13 +2264,13 @@
     </row>
     <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
@@ -2253,13 +2281,13 @@
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
@@ -2270,13 +2298,13 @@
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
@@ -2287,13 +2315,13 @@
     </row>
     <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -2304,13 +2332,13 @@
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -2321,30 +2349,30 @@
     </row>
     <row r="17" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>20</v>
@@ -2355,13 +2383,13 @@
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>21</v>
@@ -2372,172 +2400,172 @@
     </row>
     <row r="20" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D23" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="E23" s="28" t="s">
         <v>375</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -2586,79 +2614,79 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2690,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2718,23 +2746,25 @@
       <c r="A2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>452</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>57</v>
@@ -2743,48 +2773,64 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="5">
-        <v>587</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="B7" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="5">
+        <v>587</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>171</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{EA35456F-8910-A447-A530-A1B5920653C2}"/>
+    <hyperlink ref="B6" r:id="rId1" display="http://smtp.tem.scaleway.com/" xr:uid="{6EDE2DD2-A6CD-3D4D-B320-6FAADC2F5DC0}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{371A2B87-4E5B-6347-8EDA-8E7AF5F5AA5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2810,10 +2856,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>77</v>
@@ -2824,70 +2870,70 @@
     </row>
     <row r="2" spans="1:5" ht="365" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>76</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>330</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>382</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>383</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>385</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -2935,288 +2981,288 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3243,7 +3289,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3251,288 +3297,288 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>116</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>213</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>216</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="21" t="s">
         <v>269</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3572,19 +3618,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3621,64 +3667,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -3705,123 +3751,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -3848,89 +3894,89 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>176</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -3944,7 +3990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
@@ -3972,28 +4018,28 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>61</v>
@@ -4008,7 +4054,7 @@
         <v>66</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>7</v>
@@ -4028,49 +4074,49 @@
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>133</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -4078,52 +4124,52 @@
         <v>62</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>79</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -4134,49 +4180,49 @@
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>73</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -4187,49 +4233,49 @@
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>54</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>74</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -4240,172 +4286,172 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -4413,78 +4459,78 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="N9" s="33" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O9" s="25" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="P9" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P10" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -4495,40 +4541,40 @@
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>218</v>
-      </c>
       <c r="M11" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>36</v>
@@ -4537,113 +4583,113 @@
         <v>70</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="M12" t="s">
+        <v>334</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="O12" s="7" t="s">
         <v>368</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="M12" t="s">
-        <v>337</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>371</v>
       </c>
       <c r="P12" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="N13" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="O13" s="7" t="s">
         <v>363</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="M13" s="27" t="s">
-        <v>336</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>366</v>
       </c>
       <c r="P13" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -4651,43 +4697,43 @@
         <v>60</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H14" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>102</v>
-      </c>
       <c r="I14" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>42</v>
@@ -4696,92 +4742,92 @@
         <v>70</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>37</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="P15" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N16" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="P16" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -4792,25 +4838,25 @@
         <v>4</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>65</v>
@@ -4819,22 +4865,22 @@
         <v>79</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P17" s="7" t="s">
         <v>69</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4894,10 +4940,10 @@
     </row>
     <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -4906,7 +4952,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -4936,7 +4982,7 @@
         <v>50</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>52</v>
@@ -4947,10 +4993,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -4958,7 +5004,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>46</v>
@@ -4969,10 +5015,10 @@
         <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -4980,10 +5026,10 @@
         <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -4991,10 +5037,10 @@
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>